<commit_message>
Completed Product and Sprint Backlog
Might need to be edited if development progress is made after this date.
</commit_message>
<xml_diff>
--- a/Documents/Deliverable_3/CSwap_Deliverable_3_SprintBacklog.xlsx
+++ b/Documents/Deliverable_3/CSwap_Deliverable_3_SprintBacklog.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tonyc\Documents\GitHub\COS420_Project\Documents\Deliverable_3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\School_Work\College\Computer_Science\COS420\Group\GitHub\Documents\Deliverable_3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1DE2DD1F-59A1-4068-9EC7-629B457F4AE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3828BDEA-1531-424E-8EEB-4AD60AF3D85D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sprint 1" sheetId="1" state="hidden" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="37">
   <si>
     <t>ID</t>
   </si>
@@ -118,6 +118,27 @@
   </si>
   <si>
     <t>Learn about Facebook account authorization</t>
+  </si>
+  <si>
+    <t>As an authorized user I want to navigate to a book section so that I can buy books.</t>
+  </si>
+  <si>
+    <t>As an authorized user I want to be able to create a listing so that other users can see my books.</t>
+  </si>
+  <si>
+    <t>Navigate to Books</t>
+  </si>
+  <si>
+    <t>Create a listing for books</t>
+  </si>
+  <si>
+    <t>Listing System</t>
+  </si>
+  <si>
+    <t>Anthony, Landon</t>
+  </si>
+  <si>
+    <t>Cedric, Anthony</t>
   </si>
 </sst>
 </file>
@@ -350,7 +371,7 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{9ECFD424-8CF1-42FB-8D5F-DD95CE605177}" name="Table_15" displayName="Table_15" ref="A1:I6">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{9ECFD424-8CF1-42FB-8D5F-DD95CE605177}" name="Table_15" displayName="Table_15" ref="A1:I3">
   <tableColumns count="9">
     <tableColumn id="1" xr3:uid="{0C90C078-C054-4227-9091-C28BAFE691AF}" name="ID"/>
     <tableColumn id="2" xr3:uid="{9F8707D6-34E3-4CEF-B0F1-DAD2AD71531B}" name="User Story"/>
@@ -570,20 +591,20 @@
       <selection activeCell="E6" sqref="A1:E6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.25" customWidth="1"/>
-    <col min="2" max="2" width="81.58203125" customWidth="1"/>
-    <col min="3" max="3" width="35.83203125" customWidth="1"/>
+    <col min="2" max="2" width="81.625" customWidth="1"/>
+    <col min="3" max="3" width="35.875" customWidth="1"/>
     <col min="4" max="4" width="13" customWidth="1"/>
     <col min="5" max="5" width="43.25" customWidth="1"/>
-    <col min="6" max="6" width="9.58203125" customWidth="1"/>
+    <col min="6" max="6" width="9.625" customWidth="1"/>
     <col min="7" max="7" width="10.75" customWidth="1"/>
-    <col min="8" max="8" width="19.58203125" customWidth="1"/>
+    <col min="8" max="8" width="19.625" customWidth="1"/>
     <col min="9" max="9" width="30.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -612,7 +633,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>0</v>
       </c>
@@ -641,7 +662,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
         <v>1</v>
       </c>
@@ -670,7 +691,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>2</v>
       </c>
@@ -699,7 +720,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
         <v>3</v>
       </c>
@@ -728,7 +749,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>4</v>
       </c>
@@ -774,20 +795,20 @@
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.33203125" customWidth="1"/>
+    <col min="1" max="1" width="4.375" customWidth="1"/>
     <col min="2" max="2" width="40.75" customWidth="1"/>
-    <col min="3" max="3" width="35.6640625" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" customWidth="1"/>
-    <col min="5" max="5" width="15.58203125" customWidth="1"/>
+    <col min="3" max="3" width="35.625" customWidth="1"/>
+    <col min="4" max="4" width="14.625" customWidth="1"/>
+    <col min="5" max="5" width="15.625" customWidth="1"/>
     <col min="6" max="6" width="11.25" customWidth="1"/>
-    <col min="7" max="7" width="14.6640625" customWidth="1"/>
-    <col min="8" max="8" width="21.83203125" customWidth="1"/>
-    <col min="9" max="9" width="32.4140625" customWidth="1"/>
+    <col min="7" max="7" width="14.625" customWidth="1"/>
+    <col min="8" max="8" width="21.875" customWidth="1"/>
+    <col min="9" max="9" width="32.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
@@ -816,7 +837,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="10">
         <v>0</v>
       </c>
@@ -845,7 +866,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="10">
         <v>1</v>
       </c>
@@ -874,7 +895,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="10">
         <v>2</v>
       </c>
@@ -903,7 +924,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="10">
         <v>3</v>
       </c>
@@ -932,7 +953,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="24" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" ht="36.75" x14ac:dyDescent="0.25">
       <c r="A6" s="10">
         <v>4</v>
       </c>
@@ -974,20 +995,20 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="B39" sqref="B39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="10.58203125" customWidth="1"/>
-    <col min="2" max="2" width="84.58203125" customWidth="1"/>
+    <col min="1" max="1" width="10.625" customWidth="1"/>
+    <col min="2" max="2" width="84.625" customWidth="1"/>
     <col min="3" max="3" width="38.5" customWidth="1"/>
     <col min="4" max="4" width="14" customWidth="1"/>
     <col min="5" max="5" width="21.25" customWidth="1"/>
-    <col min="6" max="26" width="10.58203125" customWidth="1"/>
+    <col min="6" max="26" width="10.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -1004,7 +1025,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="15">
         <v>0</v>
       </c>
@@ -1021,7 +1042,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="19">
         <v>1</v>
       </c>
@@ -1038,7 +1059,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="15">
         <v>2</v>
       </c>
@@ -1055,7 +1076,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="19">
         <v>3</v>
       </c>
@@ -1072,7 +1093,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="15">
         <v>4</v>
       </c>
@@ -1097,28 +1118,28 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A71F075-EA9E-4381-85F8-B2F73BB54DDD}">
-  <dimension ref="A1:I6"/>
+  <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.83203125" customWidth="1"/>
-    <col min="3" max="3" width="19.1640625" customWidth="1"/>
-    <col min="4" max="4" width="26.08203125" customWidth="1"/>
-    <col min="5" max="6" width="14.58203125" customWidth="1"/>
-    <col min="7" max="7" width="15.4140625" customWidth="1"/>
-    <col min="8" max="8" width="18.4140625" customWidth="1"/>
-    <col min="9" max="9" width="43.4140625" customWidth="1"/>
+    <col min="2" max="2" width="70" customWidth="1"/>
+    <col min="3" max="3" width="22.5" customWidth="1"/>
+    <col min="4" max="4" width="17" customWidth="1"/>
+    <col min="5" max="6" width="14.625" customWidth="1"/>
+    <col min="7" max="7" width="11.875" customWidth="1"/>
+    <col min="8" max="8" width="22.75" customWidth="1"/>
+    <col min="9" max="9" width="43.375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="14" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="25" t="s">
@@ -1143,60 +1164,63 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A2" s="10"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="26"/>
-      <c r="D2" s="8"/>
-      <c r="E2" s="26"/>
-      <c r="F2" s="25"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="8"/>
-      <c r="I2" s="9"/>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A3" s="10"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="26"/>
-      <c r="D3" s="8"/>
-      <c r="E3" s="26"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="8"/>
-      <c r="I3" s="9"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A4" s="10"/>
-      <c r="B4" s="3"/>
-      <c r="C4" s="26"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="26"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="8"/>
-      <c r="I4" s="9"/>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
-      <c r="A5" s="10"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="26"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="26"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="8"/>
-      <c r="I5" s="9"/>
-    </row>
-    <row r="6" spans="1:9" ht="36.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="10"/>
-      <c r="B6" s="12"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="25"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="25"/>
-      <c r="I6" s="27"/>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="10">
+        <v>0</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="26" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="8">
+        <v>3</v>
+      </c>
+      <c r="E2" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="8">
+        <v>3</v>
+      </c>
+      <c r="H2" s="8">
+        <v>1.5</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="10">
+        <v>1</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="C3" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D3" s="8">
+        <v>3</v>
+      </c>
+      <c r="E3" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="25" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="8">
+        <v>2</v>
+      </c>
+      <c r="H3" s="8">
+        <v>1</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>36</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>